<commit_message>
Article + Font Change
</commit_message>
<xml_diff>
--- a/data/fun_fact.xlsx
+++ b/data/fun_fact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Alex and Pedro Stuff\alexandpedro.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC7FAF44-262A-4706-8932-EC5471D2804B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA2CE7B-6C71-4620-8A25-D94D5DFD1CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{63D93FC5-D3FB-4CA8-91DA-CAA838F4A3E5}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>Pangil's realname is only known by a handful of animals.</t>
-  </si>
-  <si>
     <t>Pedro have a school classroom and a part of his bedroom dedicated to research of Pawesome's secret identity.</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Pawesome made a first appearance at San Juanito City when Pedro was still in high school.</t>
+  </si>
+  <si>
+    <t>Pangil's truename is only known by a handful of animals.</t>
   </si>
 </sst>
 </file>
@@ -476,77 +476,77 @@
   <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>